<commit_message>
Fixed object translation metric
</commit_message>
<xml_diff>
--- a/scripts/Output.xlsx
+++ b/scripts/Output.xlsx
@@ -1,52 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time - T8" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T2" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T3" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T4" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T5" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T6" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T7" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeSpentIdle - T8" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T2" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T3" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T4" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T5" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T6" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T7" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalObjectTranslation - T8" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T1" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T2" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T3" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T4" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T5" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T6" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T7" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalMovement - T8" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T1" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T2" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T3" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T4" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T5" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T6" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T7" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TotalTranslationMovement - T8" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="Time - T1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Time - T2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Time - T3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Time - T4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Time - T5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Time - T6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Time - T7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Time - T8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="TimeSpentIdle - T1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="TimeSpentIdle - T2" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="TimeSpentIdle - T3" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TimeSpentIdle - T4" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="TimeSpentIdle - T5" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="TimeSpentIdle - T6" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="TimeSpentIdle - T7" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="TimeSpentIdle - T8" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="TotalObjectTranslation - T1" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="TotalObjectTranslation - T2" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="TotalObjectTranslation - T3" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="TotalObjectTranslation - T4" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="TotalObjectTranslation - T5" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TotalObjectTranslation - T6" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TotalObjectTranslation - T7" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="TotalObjectTranslation - T8" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TotalMovement - T1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="TotalMovement - T2" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="TotalMovement - T3" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="TotalMovement - T4" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="TotalMovement - T5" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="TotalMovement - T6" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="TotalMovement - T7" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="TotalMovement - T8" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="TotalTranslationMovement - T1" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="TotalTranslationMovement - T2" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="TotalTranslationMovement - T3" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="TotalTranslationMovement - T4" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="TotalTranslationMovement - T5" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="TotalTranslationMovement - T6" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="TotalTranslationMovement - T7" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="TotalTranslationMovement - T8" sheetId="40" state="visible" r:id="rId40"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3125,7 +3125,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.011780608630152</v>
+        <v>1.07</v>
       </c>
       <c r="C7" t="n">
         <v>1.25</v>
@@ -3180,7 +3180,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9773944955850733</v>
+        <v>1.09</v>
       </c>
       <c r="C12" t="n">
         <v>1.17</v>
@@ -3191,7 +3191,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.480979405663698</v>
+        <v>1.65</v>
       </c>
       <c r="C13" t="n">
         <v>1.4</v>
@@ -3202,7 +3202,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1.058489489791939</v>
+        <v>1.38</v>
       </c>
       <c r="C14" t="n">
         <v>1.01</v>
@@ -3213,7 +3213,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9176055797563569</v>
+        <v>1.14</v>
       </c>
       <c r="C15" t="n">
         <v>1.51</v>
@@ -3246,7 +3246,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1.270590413941487</v>
+        <v>1.72</v>
       </c>
       <c r="C18" t="n">
         <v>2.31</v>
@@ -3290,7 +3290,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.8820430828479978</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C22" t="n">
         <v>1.24</v>
@@ -3392,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.607980099379342</v>
+        <v>1.76</v>
       </c>
       <c r="C2" t="n">
         <v>1.87</v>
@@ -3403,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1.335402561027947</v>
+        <v>1.45</v>
       </c>
       <c r="C3" t="n">
         <v>7.33</v>
@@ -3414,7 +3414,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.661202735606591</v>
+        <v>2.74</v>
       </c>
       <c r="C4" t="n">
         <v>2.12</v>
@@ -3425,7 +3425,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>10.30069900540735</v>
+        <v>10.42</v>
       </c>
       <c r="C5" t="n">
         <v>1.95</v>
@@ -3436,7 +3436,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1.231015840677934</v>
+        <v>1.28</v>
       </c>
       <c r="C6" t="n">
         <v>1.91</v>
@@ -3447,7 +3447,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.680476123008</v>
+        <v>1.72</v>
       </c>
       <c r="C7" t="n">
         <v>1.41</v>
@@ -3458,7 +3458,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2.534284909002932</v>
+        <v>2.86</v>
       </c>
       <c r="C8" t="n">
         <v>1.37</v>
@@ -3469,7 +3469,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1.567322557739791</v>
+        <v>1.87</v>
       </c>
       <c r="C9" t="n">
         <v>1.85</v>
@@ -3480,7 +3480,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1.382316895650198</v>
+        <v>1.46</v>
       </c>
       <c r="C10" t="n">
         <v>1.91</v>
@@ -3491,7 +3491,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1.436836803537549</v>
+        <v>1.57</v>
       </c>
       <c r="C11" t="n">
         <v>3.04</v>
@@ -3502,7 +3502,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.492007223103497</v>
+        <v>2.59</v>
       </c>
       <c r="C12" t="n">
         <v>2.37</v>
@@ -3513,7 +3513,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.744133022449836</v>
+        <v>1.86</v>
       </c>
       <c r="C13" t="n">
         <v>1.38</v>
@@ -3524,7 +3524,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1.991808223700264</v>
+        <v>2.45</v>
       </c>
       <c r="C14" t="n">
         <v>2.66</v>
@@ -3535,7 +3535,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>1.54434452114805</v>
+        <v>2.04</v>
       </c>
       <c r="C15" t="n">
         <v>24.35</v>
@@ -3546,7 +3546,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>1.421724305201258</v>
+        <v>1.49</v>
       </c>
       <c r="C16" t="n">
         <v>1.97</v>
@@ -3557,7 +3557,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>1.621974105835232</v>
+        <v>1.7</v>
       </c>
       <c r="C17" t="n">
         <v>1.66</v>
@@ -3568,7 +3568,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1.394632568098135</v>
+        <v>1.7</v>
       </c>
       <c r="C18" t="n">
         <v>1.6</v>
@@ -3579,7 +3579,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1.697557068260151</v>
+        <v>1.85</v>
       </c>
       <c r="C19" t="n">
         <v>1.5</v>
@@ -3590,7 +3590,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1.234908903522847</v>
+        <v>1.34</v>
       </c>
       <c r="C20" t="n">
         <v>1.62</v>
@@ -3601,7 +3601,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>1.370583817210754</v>
+        <v>1.53</v>
       </c>
       <c r="C21" t="n">
         <v>1.68</v>
@@ -3612,7 +3612,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>1.241692393469494</v>
+        <v>1.4</v>
       </c>
       <c r="C22" t="n">
         <v>1.95</v>
@@ -3623,7 +3623,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1.422743827960606</v>
+        <v>1.6</v>
       </c>
       <c r="C23" t="n">
         <v>1.8</v>
@@ -3634,7 +3634,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>1.372953021774598</v>
+        <v>1.46</v>
       </c>
       <c r="C24" t="n">
         <v>1.82</v>
@@ -3645,7 +3645,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>1.701881311960385</v>
+        <v>1.78</v>
       </c>
       <c r="C25" t="n">
         <v>1.37</v>
@@ -3656,7 +3656,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>1.373644786689776</v>
+        <v>1.47</v>
       </c>
       <c r="C26" t="n">
         <v>1.52</v>
@@ -3667,7 +3667,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1.40089257261219</v>
+        <v>1.45</v>
       </c>
       <c r="C27" t="n">
         <v>1.5</v>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.356799283878017</v>
+        <v>5.05</v>
       </c>
       <c r="C2" t="n">
         <v>4.35</v>
@@ -3725,7 +3725,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.406890077475351</v>
+        <v>3.87</v>
       </c>
       <c r="C3" t="n">
         <v>5.82</v>
@@ -3736,7 +3736,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>4.791179395514219</v>
+        <v>5.22</v>
       </c>
       <c r="C4" t="n">
         <v>5.49</v>
@@ -3747,7 +3747,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.90486875579705</v>
+        <v>4.32</v>
       </c>
       <c r="C5" t="n">
         <v>6.13</v>
@@ -3758,7 +3758,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>4.377270839233049</v>
+        <v>4.91</v>
       </c>
       <c r="C6" t="n">
         <v>5.53</v>
@@ -3769,7 +3769,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>4.291200298284852</v>
+        <v>5.08</v>
       </c>
       <c r="C7" t="n">
         <v>4.85</v>
@@ -3780,7 +3780,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.268409399080844</v>
+        <v>3.67</v>
       </c>
       <c r="C8" t="n">
         <v>3.98</v>
@@ -3791,7 +3791,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.326619906150987</v>
+        <v>3.72</v>
       </c>
       <c r="C9" t="n">
         <v>14.37</v>
@@ -3802,7 +3802,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>3.817446790722825</v>
+        <v>4.37</v>
       </c>
       <c r="C10" t="n">
         <v>4.77</v>
@@ -3813,7 +3813,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5.19299528210839</v>
+        <v>5.88</v>
       </c>
       <c r="C11" t="n">
         <v>4.49</v>
@@ -3824,7 +3824,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>7.733724846411334</v>
+        <v>9.19</v>
       </c>
       <c r="C12" t="n">
         <v>3.79</v>
@@ -3835,7 +3835,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>3.840052082980125</v>
+        <v>4.54</v>
       </c>
       <c r="C13" t="n">
         <v>3.78</v>
@@ -3846,7 +3846,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>5.272304998764771</v>
+        <v>5.62</v>
       </c>
       <c r="C14" t="n">
         <v>5.47</v>
@@ -3857,7 +3857,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>3.555980877338909</v>
+        <v>4.08</v>
       </c>
       <c r="C15" t="n">
         <v>5.37</v>
@@ -3868,7 +3868,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>6.313984478916622</v>
+        <v>6.72</v>
       </c>
       <c r="C16" t="n">
         <v>4.35</v>
@@ -3879,7 +3879,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>4.061773011875479</v>
+        <v>4.46</v>
       </c>
       <c r="C17" t="n">
         <v>7.71</v>
@@ -3890,7 +3890,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>3.55147856533022</v>
+        <v>3.92</v>
       </c>
       <c r="C18" t="n">
         <v>6.59</v>
@@ -3901,7 +3901,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4.136302696853798</v>
+        <v>5.220000000000001</v>
       </c>
       <c r="C19" t="n">
         <v>4.31</v>
@@ -3912,7 +3912,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>3.26671088405448</v>
+        <v>3.58</v>
       </c>
       <c r="C20" t="n">
         <v>4.8</v>
@@ -3923,7 +3923,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.692654871498283</v>
+        <v>4.15</v>
       </c>
       <c r="C21" t="n">
         <v>6.96</v>
@@ -3934,7 +3934,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4.464437254570838</v>
+        <v>5.32</v>
       </c>
       <c r="C22" t="n">
         <v>4.31</v>
@@ -3945,7 +3945,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>4.370823720993561</v>
+        <v>5.41</v>
       </c>
       <c r="C23" t="n">
         <v>4.56</v>
@@ -3956,7 +3956,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>3.567408022640528</v>
+        <v>4.48</v>
       </c>
       <c r="C24" t="n">
         <v>3.61</v>
@@ -3967,7 +3967,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.657157366042648</v>
+        <v>4.140000000000001</v>
       </c>
       <c r="C25" t="n">
         <v>12.56</v>
@@ -3978,7 +3978,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>5.030516872052017</v>
+        <v>5.890000000000001</v>
       </c>
       <c r="C26" t="n">
         <v>4.17</v>
@@ -3989,7 +3989,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.701675296402968</v>
+        <v>4.08</v>
       </c>
       <c r="C27" t="n">
         <v>4.88</v>
@@ -4358,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.144980127123223</v>
+        <v>3.63</v>
       </c>
       <c r="C2" t="n">
         <v>8.779999999999999</v>
@@ -4369,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.068876015742571</v>
+        <v>3.46</v>
       </c>
       <c r="C3" t="n">
         <v>6.81</v>
@@ -4380,7 +4380,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.367565886512096</v>
+        <v>3.77</v>
       </c>
       <c r="C4" t="n">
         <v>5.28</v>
@@ -4391,7 +4391,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.357647986314229</v>
+        <v>3.76</v>
       </c>
       <c r="C5" t="n">
         <v>5.19</v>
@@ -4402,7 +4402,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.150872894929277</v>
+        <v>3.56</v>
       </c>
       <c r="C6" t="n">
         <v>4.22</v>
@@ -4413,7 +4413,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3.158053197778656</v>
+        <v>3.55</v>
       </c>
       <c r="C7" t="n">
         <v>4.16</v>
@@ -4424,7 +4424,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.6156603822815</v>
+        <v>4.02</v>
       </c>
       <c r="C8" t="n">
         <v>4.11</v>
@@ -4435,7 +4435,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.060359456011663</v>
+        <v>3.46</v>
       </c>
       <c r="C9" t="n">
         <v>4.46</v>
@@ -4446,7 +4446,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4.053492321443325</v>
+        <v>4.539999999999999</v>
       </c>
       <c r="C10" t="n">
         <v>3.99</v>
@@ -4457,7 +4457,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>3.419736831979912</v>
+        <v>3.84</v>
       </c>
       <c r="C11" t="n">
         <v>4.95</v>
@@ -4468,7 +4468,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.503041535580188</v>
+        <v>3.95</v>
       </c>
       <c r="C12" t="n">
         <v>5.37</v>
@@ -4479,7 +4479,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>3.0886890422961</v>
+        <v>3.48</v>
       </c>
       <c r="C13" t="n">
         <v>4.14</v>
@@ -4490,7 +4490,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>3.830469945058961</v>
+        <v>4.79</v>
       </c>
       <c r="C14" t="n">
         <v>6.28</v>
@@ -4501,7 +4501,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>3.140971187387748</v>
+        <v>3.55</v>
       </c>
       <c r="C15" t="n">
         <v>5.48</v>
@@ -4512,7 +4512,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>3.23579974658507</v>
+        <v>3.68</v>
       </c>
       <c r="C16" t="n">
         <v>4.46</v>
@@ -4523,7 +4523,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>3.216364407215078</v>
+        <v>3.8</v>
       </c>
       <c r="C17" t="n">
         <v>5.29</v>
@@ -4534,7 +4534,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>4.673692330481329</v>
+        <v>5.12</v>
       </c>
       <c r="C18" t="n">
         <v>6.26</v>
@@ -4545,7 +4545,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>3.162182790415506</v>
+        <v>3.58</v>
       </c>
       <c r="C19" t="n">
         <v>6.31</v>
@@ -4556,7 +4556,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>3.090064724241226</v>
+        <v>3.49</v>
       </c>
       <c r="C20" t="n">
         <v>13.12</v>
@@ -4567,7 +4567,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.227444809752756</v>
+        <v>3.62</v>
       </c>
       <c r="C21" t="n">
         <v>8.220000000000001</v>
@@ -4578,7 +4578,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>3.050458981858304</v>
+        <v>3.45</v>
       </c>
       <c r="C22" t="n">
         <v>4.15</v>
@@ -4589,7 +4589,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>4.198309183468983</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="C23" t="n">
         <v>3.88</v>
@@ -4600,7 +4600,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>3.078782226790326</v>
+        <v>3.47</v>
       </c>
       <c r="C24" t="n">
         <v>3.37</v>
@@ -4611,7 +4611,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.210062304691297</v>
+        <v>4.03</v>
       </c>
       <c r="C25" t="n">
         <v>5.03</v>
@@ -4622,7 +4622,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>3.22158346159152</v>
+        <v>3.64</v>
       </c>
       <c r="C26" t="n">
         <v>4.6</v>
@@ -4633,7 +4633,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.23736003558455</v>
+        <v>3.63</v>
       </c>
       <c r="C27" t="n">
         <v>3.31</v>
@@ -4680,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>57.8669249226188</v>
+        <v>70.32000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>80.59999999999999</v>
@@ -4691,7 +4691,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>51.43173339486042</v>
+        <v>64.92</v>
       </c>
       <c r="C3" t="n">
         <v>60.83</v>
@@ -4702,7 +4702,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>37.84109538583681</v>
+        <v>46.59</v>
       </c>
       <c r="C4" t="n">
         <v>32.4</v>
@@ -4713,7 +4713,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>120.7905695822319</v>
+        <v>139.53</v>
       </c>
       <c r="C5" t="n">
         <v>39.17</v>
@@ -4724,7 +4724,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>51.18894118850282</v>
+        <v>67.65000000000001</v>
       </c>
       <c r="C6" t="n">
         <v>44.57</v>
@@ -4735,7 +4735,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>37.71424797076034</v>
+        <v>48.51000000000001</v>
       </c>
       <c r="C7" t="n">
         <v>38.43</v>
@@ -4746,7 +4746,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>49.34736568450235</v>
+        <v>62.39</v>
       </c>
       <c r="C8" t="n">
         <v>29.79</v>
@@ -4757,7 +4757,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>27.11101805539585</v>
+        <v>35.65</v>
       </c>
       <c r="C9" t="n">
         <v>36.03</v>
@@ -4768,7 +4768,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>180.7061672992928</v>
+        <v>223.53</v>
       </c>
       <c r="C10" t="n">
         <v>46.92</v>
@@ -4779,7 +4779,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>44.93768240574941</v>
+        <v>59.95</v>
       </c>
       <c r="C11" t="n">
         <v>42.71</v>
@@ -4790,7 +4790,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>30.44212870349247</v>
+        <v>40</v>
       </c>
       <c r="C12" t="n">
         <v>88.26000000000001</v>
@@ -4801,7 +4801,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>67.2030988868817</v>
+        <v>83.93000000000001</v>
       </c>
       <c r="C13" t="n">
         <v>34.62</v>
@@ -4812,7 +4812,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>50.33955105083874</v>
+        <v>62.72</v>
       </c>
       <c r="C14" t="n">
         <v>42.31</v>
@@ -4823,7 +4823,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>31.69351353195161</v>
+        <v>40.26</v>
       </c>
       <c r="C15" t="n">
         <v>1980.85</v>
@@ -4834,7 +4834,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>28.63648721474057</v>
+        <v>37.02</v>
       </c>
       <c r="C16" t="n">
         <v>35.38</v>
@@ -4845,7 +4845,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>77.47370779819435</v>
+        <v>97.48</v>
       </c>
       <c r="C17" t="n">
         <v>33.32</v>
@@ -4856,7 +4856,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>36.67301187521963</v>
+        <v>47.7</v>
       </c>
       <c r="C18" t="n">
         <v>68.12</v>
@@ -4867,7 +4867,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>29.10527100028447</v>
+        <v>38.56</v>
       </c>
       <c r="C19" t="n">
         <v>34.55</v>
@@ -4878,7 +4878,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>63.67006360920335</v>
+        <v>85.34</v>
       </c>
       <c r="C20" t="n">
         <v>33.15</v>
@@ -4889,7 +4889,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>36.56242470077716</v>
+        <v>50.53</v>
       </c>
       <c r="C21" t="n">
         <v>29.59</v>
@@ -4900,7 +4900,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>131.00757230023</v>
+        <v>148.52</v>
       </c>
       <c r="C22" t="n">
         <v>30.76</v>
@@ -4911,7 +4911,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>40.03784709496753</v>
+        <v>48.5</v>
       </c>
       <c r="C23" t="n">
         <v>43.57</v>
@@ -4922,7 +4922,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>32.70926015672015</v>
+        <v>42.75</v>
       </c>
       <c r="C24" t="n">
         <v>29.21</v>
@@ -4933,7 +4933,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>105.9827278380775</v>
+        <v>125.16</v>
       </c>
       <c r="C25" t="n">
         <v>31.79</v>
@@ -4944,7 +4944,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>41.31237223883421</v>
+        <v>51.91</v>
       </c>
       <c r="C26" t="n">
         <v>29.52</v>
@@ -4955,7 +4955,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>38.19227670616142</v>
+        <v>51.18</v>
       </c>
       <c r="C27" t="n">
         <v>30.82</v>
@@ -5002,7 +5002,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>73.78734918670003</v>
+        <v>97.33000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>93.34</v>
@@ -5013,7 +5013,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>44.6173116626271</v>
+        <v>63.09</v>
       </c>
       <c r="C3" t="n">
         <v>79.73999999999999</v>
@@ -5024,7 +5024,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>49.38387692354662</v>
+        <v>68.95</v>
       </c>
       <c r="C4" t="n">
         <v>75.95</v>
@@ -5035,7 +5035,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>55.2981753767699</v>
+        <v>76.08</v>
       </c>
       <c r="C5" t="n">
         <v>321.5</v>
@@ -5046,7 +5046,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>52.2598430919956</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="C6" t="n">
         <v>178.63</v>
@@ -5057,7 +5057,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>51.85043297794146</v>
+        <v>72.72</v>
       </c>
       <c r="C7" t="n">
         <v>71.42</v>
@@ -5068,7 +5068,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>67.43760746052607</v>
+        <v>89.23</v>
       </c>
       <c r="C8" t="n">
         <v>58.79</v>
@@ -5079,7 +5079,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>62.88367435193334</v>
+        <v>88.93000000000001</v>
       </c>
       <c r="C9" t="n">
         <v>65.98999999999999</v>
@@ -5090,7 +5090,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>77.93401118895396</v>
+        <v>105.71</v>
       </c>
       <c r="C10" t="n">
         <v>70.88</v>
@@ -5101,7 +5101,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>53.76051060025379</v>
+        <v>74.25</v>
       </c>
       <c r="C11" t="n">
         <v>59.39</v>
@@ -5112,7 +5112,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>48.09496023493522</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="C12" t="n">
         <v>57.61</v>
@@ -5123,7 +5123,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>65.05290923548307</v>
+        <v>89.22</v>
       </c>
       <c r="C13" t="n">
         <v>81.26000000000001</v>
@@ -5134,7 +5134,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>83.77587540575149</v>
+        <v>112.75</v>
       </c>
       <c r="C14" t="n">
         <v>145.77</v>
@@ -5145,7 +5145,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>65.56473594852648</v>
+        <v>89.84</v>
       </c>
       <c r="C15" t="n">
         <v>69.94</v>
@@ -5156,7 +5156,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>59.91125770671152</v>
+        <v>81.74000000000001</v>
       </c>
       <c r="C16" t="n">
         <v>957.23</v>
@@ -5167,7 +5167,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>50.39415144637321</v>
+        <v>70.83</v>
       </c>
       <c r="C17" t="n">
         <v>89.51000000000001</v>
@@ -5178,7 +5178,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>100.3637848030852</v>
+        <v>128.95</v>
       </c>
       <c r="C18" t="n">
         <v>133.37</v>
@@ -5189,7 +5189,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>81.87333204407892</v>
+        <v>109.59</v>
       </c>
       <c r="C19" t="n">
         <v>50.33</v>
@@ -5200,7 +5200,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>54.39209501388966</v>
+        <v>74</v>
       </c>
       <c r="C20" t="n">
         <v>97.33</v>
@@ -5211,7 +5211,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>55.35606290190804</v>
+        <v>75.42999999999999</v>
       </c>
       <c r="C21" t="n">
         <v>58.25</v>
@@ -5222,7 +5222,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>64.98541682562328</v>
+        <v>86.38</v>
       </c>
       <c r="C22" t="n">
         <v>82.12</v>
@@ -5233,7 +5233,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>57.31375053161327</v>
+        <v>79.34</v>
       </c>
       <c r="C23" t="n">
         <v>66.98999999999999</v>
@@ -5244,7 +5244,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>49.97503076537323</v>
+        <v>69.05</v>
       </c>
       <c r="C24" t="n">
         <v>67.3</v>
@@ -5255,7 +5255,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>44.5322175508923</v>
+        <v>62.68</v>
       </c>
       <c r="C25" t="n">
         <v>96.37</v>
@@ -5266,7 +5266,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>49.44146943609181</v>
+        <v>69.43000000000001</v>
       </c>
       <c r="C26" t="n">
         <v>53.6</v>
@@ -5277,7 +5277,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>49.15847129437611</v>
+        <v>67.75</v>
       </c>
       <c r="C27" t="n">
         <v>56.65</v>
@@ -5346,7 +5346,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>47.01758819846037</v>
+        <v>49.64</v>
       </c>
       <c r="C4" t="n">
         <v>66.34</v>
@@ -5434,7 +5434,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>51.94177990789303</v>
+        <v>52.37</v>
       </c>
       <c r="C12" t="n">
         <v>109.88</v>
@@ -5456,7 +5456,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>60.38280053127711</v>
+        <v>62.34</v>
       </c>
       <c r="C14" t="n">
         <v>145.11</v>
@@ -5467,7 +5467,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>167.3269529992105</v>
+        <v>189.22</v>
       </c>
       <c r="C15" t="n">
         <v>65.64</v>
@@ -5478,7 +5478,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>62.57002876777347</v>
+        <v>62.63</v>
       </c>
       <c r="C16" t="n">
         <v>66.84</v>
@@ -5522,7 +5522,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>64.23924423590302</v>
+        <v>68.72999999999999</v>
       </c>
       <c r="C20" t="n">
         <v>62.92</v>
@@ -5555,7 +5555,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>96.32954479286197</v>
+        <v>102.18</v>
       </c>
       <c r="C23" t="n">
         <v>55.46</v>
@@ -5588,7 +5588,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>52.14572082155927</v>
+        <v>54.5</v>
       </c>
       <c r="C26" t="n">
         <v>58.45</v>
@@ -5646,7 +5646,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>131.9648441820775</v>
+        <v>139.11</v>
       </c>
       <c r="C2" t="n">
         <v>216.18</v>
@@ -5657,7 +5657,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>127.1808869288149</v>
+        <v>143.54</v>
       </c>
       <c r="C3" t="n">
         <v>185.57</v>
@@ -5668,7 +5668,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>108.4868051884652</v>
+        <v>149.57</v>
       </c>
       <c r="C4" t="n">
         <v>232.56</v>
@@ -5679,7 +5679,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>155.4154718810196</v>
+        <v>164.23</v>
       </c>
       <c r="C5" t="n">
         <v>429.98</v>
@@ -5690,7 +5690,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>102.6090741601346</v>
+        <v>124.89</v>
       </c>
       <c r="C6" t="n">
         <v>251.34</v>
@@ -5701,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>105.9476191332302</v>
+        <v>121.02</v>
       </c>
       <c r="C7" t="n">
         <v>196.19</v>
@@ -5712,7 +5712,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>108.9654202029249</v>
+        <v>130.66</v>
       </c>
       <c r="C8" t="n">
         <v>112.02</v>
@@ -5723,7 +5723,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>100.8459126588678</v>
+        <v>116.89</v>
       </c>
       <c r="C9" t="n">
         <v>183.07</v>
@@ -5734,7 +5734,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>258.3178307821588</v>
+        <v>268.47</v>
       </c>
       <c r="C10" t="n">
         <v>176.8</v>
@@ -5745,7 +5745,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>206.8277892353927</v>
+        <v>277.68</v>
       </c>
       <c r="C11" t="n">
         <v>257.19</v>
@@ -5756,7 +5756,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>94.89680500417282</v>
+        <v>103.74</v>
       </c>
       <c r="C12" t="n">
         <v>189.41</v>
@@ -5767,7 +5767,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>111.3795479430582</v>
+        <v>140.07</v>
       </c>
       <c r="C13" t="n">
         <v>99.56</v>
@@ -5778,7 +5778,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>117.8718363308216</v>
+        <v>126</v>
       </c>
       <c r="C14" t="n">
         <v>203.93</v>
@@ -5789,7 +5789,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>131.9556535355723</v>
+        <v>154.59</v>
       </c>
       <c r="C15" t="n">
         <v>350.55</v>
@@ -5800,7 +5800,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>179.9526273773184</v>
+        <v>187.21</v>
       </c>
       <c r="C16" t="n">
         <v>137.42</v>
@@ -5811,7 +5811,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>128.6562124423069</v>
+        <v>151.26</v>
       </c>
       <c r="C17" t="n">
         <v>98.03</v>
@@ -5822,7 +5822,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>153.0750551200293</v>
+        <v>169.35</v>
       </c>
       <c r="C18" t="n">
         <v>850.9</v>
@@ -5833,7 +5833,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>105.9746597069318</v>
+        <v>114.17</v>
       </c>
       <c r="C19" t="n">
         <v>161.6</v>
@@ -5844,7 +5844,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>97.26912613979833</v>
+        <v>105.87</v>
       </c>
       <c r="C20" t="n">
         <v>191.41</v>
@@ -5855,7 +5855,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>111.3611067653335</v>
+        <v>120.51</v>
       </c>
       <c r="C21" t="n">
         <v>144.88</v>
@@ -5866,7 +5866,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>94.76141408822475</v>
+        <v>103.64</v>
       </c>
       <c r="C22" t="n">
         <v>112.88</v>
@@ -5877,7 +5877,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>123.620467560999</v>
+        <v>138.04</v>
       </c>
       <c r="C23" t="n">
         <v>160.6</v>
@@ -5888,7 +5888,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>87.43350216021317</v>
+        <v>97.45</v>
       </c>
       <c r="C24" t="n">
         <v>140.35</v>
@@ -5899,7 +5899,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>81.94800119588029</v>
+        <v>94.36999999999999</v>
       </c>
       <c r="C25" t="n">
         <v>213.86</v>
@@ -5910,7 +5910,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>129.4658395098877</v>
+        <v>146.26</v>
       </c>
       <c r="C26" t="n">
         <v>397.14</v>
@@ -5921,7 +5921,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>204.8641054455368</v>
+        <v>233.03</v>
       </c>
       <c r="C27" t="n">
         <v>126.55</v>

</xml_diff>